<commit_message>
commit on 24th april
</commit_message>
<xml_diff>
--- a/Testdata/Testdata.xlsx
+++ b/Testdata/Testdata.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15960" windowHeight="6345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CommonTestdata" sheetId="1" r:id="rId1"/>
-    <sheet name="ApplyLeave" sheetId="2" r:id="rId2"/>
+    <sheet name="Addstaff" sheetId="3" r:id="rId2"/>
+    <sheet name="Deletecustomer" sheetId="4" r:id="rId3"/>
+    <sheet name="Deletestaff" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Sno</t>
   </si>
@@ -40,65 +42,95 @@
     <t>QA</t>
   </si>
   <si>
-    <t>http://testingmasters.com/hrm</t>
-  </si>
-  <si>
-    <t>user01</t>
+    <t>Tc_Name</t>
+  </si>
+  <si>
+    <t>Iteration</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Tc_01_AddStaff</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>DOJ</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Mani</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
   </si>
   <si>
     <t>pass1234</t>
   </si>
   <si>
-    <t>Tc_01_ValidateLoginCredentials</t>
-  </si>
-  <si>
-    <t>Tc_Name</t>
-  </si>
-  <si>
-    <t>Iteration</t>
-  </si>
-  <si>
-    <t>Leave_Type</t>
-  </si>
-  <si>
-    <t>From_Date</t>
-  </si>
-  <si>
-    <t>To_Date</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Personal Leave</t>
-  </si>
-  <si>
-    <t>Annual Leave</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>Testing1</t>
-  </si>
-  <si>
-    <t>Testing2</t>
-  </si>
-  <si>
-    <t>Testing3</t>
-  </si>
-  <si>
-    <t>Tc_02_VerifyLeave</t>
-  </si>
-  <si>
-    <t>2017-12-08</t>
+    <t>Staffname</t>
+  </si>
+  <si>
+    <t>http://server/bank</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>vijay</t>
+  </si>
+  <si>
+    <t>married</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>Tc_01_Deletestaff</t>
+  </si>
+  <si>
+    <t>Tc_01_deletecustomer</t>
+  </si>
+  <si>
+    <t>Manimmmbdhb@gmail.com</t>
+  </si>
+  <si>
+    <t>Manimbyhbmmbdhb@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,9 +199,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -225,7 +263,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -260,7 +298,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -437,28 +475,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -483,273 +521,294 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3">
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3">
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3">
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3">
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3">
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3">
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3">
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3">
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3">
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3">
       <c r="C26" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{D92607C3-A138-4238-B302-41830DA2C6A5}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DFCBC5-818F-4531-96EB-B86E81209CCD}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4">
+        <v>34559</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="4">
+        <v>43163</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="3">
+        <v>9874563212</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="4">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="4">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>21</v>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>